<commit_message>
Se agrego las caracteristicas para obtener y crear nuevos procesos de compra
</commit_message>
<xml_diff>
--- a/front-end-sistema/public/Formato.xlsx
+++ b/front-end-sistema/public/Formato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5710E4DC-D715-4858-904C-5BE07A2C9EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E5E696-58FB-4542-8AFF-8650E99B6D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{57AA1E4C-8E77-478E-8A74-B73F9B3EB534}"/>
   </bookViews>
@@ -17,13 +17,13 @@
     <sheet name="Datos" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Categorias">Datos!$B$3:$B$4</definedName>
-    <definedName name="MARCAS_INF">Datos!$G$3:$G$7</definedName>
-    <definedName name="MARCAS_OFI">Datos!$H$3:$H$7</definedName>
-    <definedName name="Procesos">Datos!$L$3</definedName>
-    <definedName name="TIPOS_INF">Datos!$D$3:$D$6</definedName>
-    <definedName name="TIPOS_OFI">Datos!$E$3</definedName>
-    <definedName name="UBICACIONES">Datos!$J$3</definedName>
+    <definedName name="Categorias">Tabla2[Categorias]</definedName>
+    <definedName name="MARCAS_INF">Tabla6[Marcas_Inf]</definedName>
+    <definedName name="MARCAS_OFI">Tabla5[Marcas_Ofi]</definedName>
+    <definedName name="Procesos">Tabla8[Procesos]</definedName>
+    <definedName name="TIPOS_INF">Tabla3[Tipos_Inf]</definedName>
+    <definedName name="TIPOS_OFI">Tabla7[Tipos_Ofi]</definedName>
+    <definedName name="UBICACIONES">Tabla4[Ubicaciones]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Categoria</t>
   </si>
@@ -141,7 +141,46 @@
     <t>1 - PR0001</t>
   </si>
   <si>
-    <t>3 - Fisei-Piso1-Laboratorio CTT</t>
+    <t>5 - Fisei - Piso1 - Laboratorio Redes</t>
+  </si>
+  <si>
+    <t>3 - Fisei - Piso1 - Laboratorio CTT</t>
+  </si>
+  <si>
+    <t>6 - Fisei - Piso2 - Laboratorio Redes 02</t>
+  </si>
+  <si>
+    <t>7 - Fisei - Piso3 - Administración</t>
+  </si>
+  <si>
+    <t>8 - Fisei - Piso1 - Coordinación</t>
+  </si>
+  <si>
+    <t>9 - Fche - Piso1 - Coordinación</t>
+  </si>
+  <si>
+    <t>10 - Fche - Piso1 - Laboratorio 1</t>
+  </si>
+  <si>
+    <t>11 - Fcial - Piso1 - Laboratorio Central</t>
+  </si>
+  <si>
+    <t>12 - Fcial - Piso1 - Laboratorio Bacteriologo</t>
+  </si>
+  <si>
+    <t>13 - Fcial - Piso2 - Laboratorio 05</t>
+  </si>
+  <si>
+    <t>2 - PR0002</t>
+  </si>
+  <si>
+    <t>3 - PR0003</t>
+  </si>
+  <si>
+    <t>4 - PR0004</t>
+  </si>
+  <si>
+    <t>5 - PR0005</t>
   </si>
 </sst>
 </file>
@@ -242,8 +281,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E08F9CBB-79FA-4ED8-99F3-3C73D03F831B}" name="Tabla4" displayName="Tabla4" ref="J2:J3" totalsRowShown="0">
-  <autoFilter ref="J2:J3" xr:uid="{E08F9CBB-79FA-4ED8-99F3-3C73D03F831B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E08F9CBB-79FA-4ED8-99F3-3C73D03F831B}" name="Tabla4" displayName="Tabla4" ref="J2:J12" totalsRowShown="0">
+  <autoFilter ref="J2:J12" xr:uid="{E08F9CBB-79FA-4ED8-99F3-3C73D03F831B}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{CB5BCE48-0872-4A1D-BFE2-656C4D410B39}" name="Ubicaciones"/>
   </tableColumns>
@@ -282,8 +321,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B460A981-800F-414D-AC10-A61AB0983FC9}" name="Tabla8" displayName="Tabla8" ref="L2:L3" totalsRowShown="0">
-  <autoFilter ref="L2:L3" xr:uid="{B460A981-800F-414D-AC10-A61AB0983FC9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B460A981-800F-414D-AC10-A61AB0983FC9}" name="Tabla8" displayName="Tabla8" ref="L2:L7" totalsRowShown="0">
+  <autoFilter ref="L2:L7" xr:uid="{B460A981-800F-414D-AC10-A61AB0983FC9}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{13CC3AF1-6ABF-4FFE-AE09-DF89BAC539D4}" name="Procesos"/>
   </tableColumns>
@@ -611,7 +650,7 @@
   <dimension ref="A2:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +658,7 @@
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
   </cols>
@@ -649,11 +688,11 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erroneos" error="Elige un dato que este disponible en la lista_x000a_" sqref="A3:A20" xr:uid="{6C61E344-F992-4D20-9B18-B7C1FBE67B3C}">
       <formula1>Categorias</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erroneos" error="Elige un dato que este disponible en la lista" sqref="D3:D20" xr:uid="{2BC676EE-BB0D-41B2-96D2-41AD5C5F4138}">
-      <formula1>UBICACIONES</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F20" xr:uid="{CDF91FE7-80AB-488D-9ADF-E2012E0C378A}">
       <formula1>Procesos</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erroneos" error="Elige un dato que este disponible en la lista" sqref="D5:D20 D3" xr:uid="{2BC676EE-BB0D-41B2-96D2-41AD5C5F4138}">
+      <formula1>UBICACIONES</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -693,17 +732,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1DBF0D0-2E71-4175-9FA5-5DB06734B8A1}">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="10" max="10" width="26" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
@@ -746,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
@@ -765,6 +804,12 @@
       <c r="H4" t="s">
         <v>20</v>
       </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
@@ -776,6 +821,12 @@
       <c r="H5" t="s">
         <v>21</v>
       </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
@@ -787,6 +838,12 @@
       <c r="H6" t="s">
         <v>22</v>
       </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G7" t="s">
@@ -794,6 +851,37 @@
       </c>
       <c r="H7" t="s">
         <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>